<commit_message>
some formating and details
</commit_message>
<xml_diff>
--- a/00_project_info/FinalProjectMetadata.xlsx
+++ b/00_project_info/FinalProjectMetadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderdavis/UW/Classes/info_330su/FinalProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderdavis/UW/Classes/info_330su/healthcareDB/00_project_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1224C5-F1EA-EF4F-AF86-1E7BD89B70E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531CA9B2-7209-4548-9D62-92F23E7B429E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="94">
   <si>
     <t>DataType</t>
   </si>
@@ -305,13 +305,16 @@
   </si>
   <si>
     <t>Public can view clinic info; sans ID</t>
+  </si>
+  <si>
+    <t>Patient Appointments Project</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,8 +336,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +381,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -384,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -392,7 +408,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -403,6 +418,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC32D67-99DD-1947-BCAB-073881641D79}">
-  <dimension ref="A1:F125"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:F33"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -734,97 +758,84 @@
     <col min="6" max="6" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
+      <c r="E4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -832,13 +843,13 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -846,49 +857,44 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>23</v>
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -896,24 +902,32 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1</v>
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -921,10 +935,13 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -932,7 +949,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -943,10 +960,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -954,57 +971,48 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>23</v>
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>27</v>
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1012,13 +1020,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>27</v>
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1026,7 +1037,7 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -1040,10 +1051,10 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>27</v>
@@ -1054,29 +1065,27 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>23</v>
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1084,27 +1093,29 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>27</v>
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1112,10 +1123,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>27</v>
@@ -1126,7 +1137,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
@@ -1140,10 +1151,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>27</v>
@@ -1154,29 +1165,27 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>23</v>
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1184,98 +1193,100 @@
         <v>28</v>
       </c>
       <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
         <v>7</v>
       </c>
-      <c r="C32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B35" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F33" s="5"/>
-    </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2" t="s">
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
-        <v>19</v>
-      </c>
+      <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="F38" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1283,7 +1294,7 @@
         <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
@@ -1297,7 +1308,7 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
@@ -1311,13 +1322,13 @@
         <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1325,7 +1336,7 @@
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
@@ -1339,16 +1350,13 @@
         <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1356,32 +1364,30 @@
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C44" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="D44" t="s">
         <v>19</v>
       </c>
-      <c r="F44" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>23</v>
+      <c r="A45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1389,24 +1395,32 @@
         <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C46" t="s">
-        <v>14</v>
+        <v>43</v>
+      </c>
+      <c r="D46" t="s">
+        <v>19</v>
       </c>
       <c r="F46" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" t="s">
-        <v>1</v>
+      <c r="A47" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1414,10 +1428,13 @@
         <v>13</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C48" t="s">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="F48" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1425,7 +1442,7 @@
         <v>13</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>
@@ -1436,7 +1453,7 @@
         <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C50" t="s">
         <v>1</v>
@@ -1447,7 +1464,7 @@
         <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
         <v>1</v>
@@ -1458,7 +1475,7 @@
         <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C52" t="s">
         <v>1</v>
@@ -1469,10 +1486,10 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C53" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -1480,60 +1497,48 @@
         <v>13</v>
       </c>
       <c r="B54" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C54" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>23</v>
+      <c r="A55" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B56" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C56" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" t="s">
-        <v>52</v>
-      </c>
-      <c r="F56" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>28</v>
-      </c>
-      <c r="B57" t="s">
-        <v>44</v>
-      </c>
-      <c r="C57" t="s">
-        <v>1</v>
-      </c>
-      <c r="D57" t="s">
-        <v>19</v>
-      </c>
-      <c r="F57" s="12" t="s">
-        <v>85</v>
+      <c r="A57" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -1541,22 +1546,24 @@
         <v>28</v>
       </c>
       <c r="B58" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C58" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D58" t="s">
-        <v>19</v>
-      </c>
-      <c r="F58" s="12"/>
+        <v>52</v>
+      </c>
+      <c r="F58" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>28</v>
       </c>
       <c r="B59" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C59" t="s">
         <v>1</v>
@@ -1564,13 +1571,16 @@
       <c r="D59" t="s">
         <v>19</v>
       </c>
+      <c r="F59" s="11" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>28</v>
       </c>
       <c r="B60" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C60" t="s">
         <v>1</v>
@@ -1578,19 +1588,20 @@
       <c r="D60" t="s">
         <v>19</v>
       </c>
+      <c r="F60" s="11"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>28</v>
       </c>
       <c r="B61" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C61" t="s">
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -1598,7 +1609,7 @@
         <v>28</v>
       </c>
       <c r="B62" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C62" t="s">
         <v>1</v>
@@ -1612,13 +1623,13 @@
         <v>28</v>
       </c>
       <c r="B63" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C63" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -1626,29 +1637,27 @@
         <v>28</v>
       </c>
       <c r="B64" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C64" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="D64" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>23</v>
+      <c r="A65" t="s">
+        <v>28</v>
+      </c>
+      <c r="B65" t="s">
+        <v>50</v>
+      </c>
+      <c r="C65" t="s">
+        <v>70</v>
+      </c>
+      <c r="D65" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -1656,30 +1665,29 @@
         <v>28</v>
       </c>
       <c r="B66" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C66" t="s">
-        <v>14</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F66" t="s">
-        <v>86</v>
+        <v>43</v>
+      </c>
+      <c r="D66" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>28</v>
-      </c>
-      <c r="B67" t="s">
-        <v>44</v>
-      </c>
-      <c r="C67" t="s">
-        <v>1</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>27</v>
+      <c r="A67" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -1687,13 +1695,16 @@
         <v>28</v>
       </c>
       <c r="B68" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C68" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="F68" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -1701,7 +1712,7 @@
         <v>28</v>
       </c>
       <c r="B69" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C69" t="s">
         <v>1</v>
@@ -1715,7 +1726,7 @@
         <v>28</v>
       </c>
       <c r="B70" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
@@ -1729,13 +1740,13 @@
         <v>28</v>
       </c>
       <c r="B71" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C71" t="s">
         <v>1</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -1743,7 +1754,7 @@
         <v>28</v>
       </c>
       <c r="B72" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C72" t="s">
         <v>1</v>
@@ -1757,13 +1768,13 @@
         <v>28</v>
       </c>
       <c r="B73" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C73" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -1771,29 +1782,27 @@
         <v>28</v>
       </c>
       <c r="B74" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C74" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>23</v>
+      <c r="A75" t="s">
+        <v>28</v>
+      </c>
+      <c r="B75" t="s">
+        <v>50</v>
+      </c>
+      <c r="C75" t="s">
+        <v>70</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -1801,114 +1810,114 @@
         <v>28</v>
       </c>
       <c r="B76" t="s">
+        <v>51</v>
+      </c>
+      <c r="C76" t="s">
+        <v>43</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>28</v>
+      </c>
+      <c r="B78" t="s">
         <v>42</v>
       </c>
-      <c r="C76" t="s">
-        <v>14</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="5" t="s">
+      <c r="C78" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B79" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C79" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D77" s="6" t="s">
+      <c r="D79" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E77" s="5" t="s">
+      <c r="E79" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F77" s="5"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="8"/>
-      <c r="B78" s="8"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8"/>
-      <c r="F78" s="8"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="7"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2" t="s">
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F79" s="2"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>13</v>
-      </c>
-      <c r="B80" t="s">
-        <v>55</v>
-      </c>
-      <c r="C80" t="s">
-        <v>14</v>
-      </c>
-      <c r="D80" t="s">
-        <v>18</v>
-      </c>
-      <c r="F80" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>13</v>
-      </c>
-      <c r="B81" t="s">
-        <v>56</v>
-      </c>
-      <c r="C81" t="s">
-        <v>1</v>
-      </c>
-      <c r="D81" t="s">
-        <v>19</v>
-      </c>
+      <c r="F81" s="2"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>13</v>
       </c>
       <c r="B82" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C82" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D82" t="s">
+        <v>18</v>
+      </c>
+      <c r="F82" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>13</v>
+      </c>
+      <c r="B83" t="s">
+        <v>56</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1</v>
+      </c>
+      <c r="D83" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -1916,83 +1925,82 @@
         <v>13</v>
       </c>
       <c r="B84" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C84" t="s">
-        <v>14</v>
-      </c>
-      <c r="F84" s="12" t="s">
-        <v>87</v>
+        <v>1</v>
+      </c>
+      <c r="D84" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>13</v>
-      </c>
-      <c r="B85" t="s">
-        <v>56</v>
-      </c>
-      <c r="C85" t="s">
-        <v>1</v>
-      </c>
-      <c r="F85" s="12"/>
+      <c r="A85" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>13</v>
       </c>
       <c r="B86" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C86" t="s">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="F86" s="11" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="A87" t="s">
+        <v>13</v>
+      </c>
+      <c r="B87" t="s">
+        <v>56</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1</v>
+      </c>
+      <c r="F87" s="11"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B88" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C88" t="s">
-        <v>14</v>
-      </c>
-      <c r="D88" t="s">
-        <v>52</v>
-      </c>
-      <c r="F88" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>28</v>
-      </c>
-      <c r="B89" t="s">
-        <v>56</v>
-      </c>
-      <c r="C89" t="s">
-        <v>1</v>
-      </c>
-      <c r="D89" t="s">
-        <v>19</v>
+      <c r="A89" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -2000,29 +2008,30 @@
         <v>28</v>
       </c>
       <c r="B90" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C90" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D90" t="s">
+        <v>52</v>
+      </c>
+      <c r="F90" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>28</v>
+      </c>
+      <c r="B91" t="s">
+        <v>56</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1</v>
+      </c>
+      <c r="D91" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -2030,27 +2039,29 @@
         <v>28</v>
       </c>
       <c r="B92" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C92" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D92" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>28</v>
-      </c>
-      <c r="B93" t="s">
-        <v>56</v>
-      </c>
-      <c r="C93" t="s">
-        <v>1</v>
-      </c>
-      <c r="D93" t="s">
-        <v>19</v>
+      <c r="A93" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -2058,29 +2069,27 @@
         <v>28</v>
       </c>
       <c r="B94" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C94" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D94" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>28</v>
+      </c>
+      <c r="B95" t="s">
+        <v>56</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1</v>
+      </c>
+      <c r="D95" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -2088,98 +2097,100 @@
         <v>28</v>
       </c>
       <c r="B96" t="s">
+        <v>57</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1</v>
+      </c>
+      <c r="D96" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>28</v>
+      </c>
+      <c r="B98" t="s">
         <v>55</v>
       </c>
-      <c r="C96" t="s">
-        <v>14</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="5" t="s">
+      <c r="C98" t="s">
+        <v>14</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B99" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C97" s="5" t="s">
+      <c r="C99" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D97" s="6" t="s">
+      <c r="D99" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E97" s="5" t="s">
+      <c r="E99" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F97" s="5"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="8"/>
-      <c r="B98" s="8"/>
-      <c r="C98" s="8"/>
-      <c r="D98" s="8"/>
-      <c r="E98" s="8"/>
-      <c r="F98" s="8"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="2" t="s">
+      <c r="F99" s="5"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="7"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="7"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="7"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2" t="s">
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F99" s="2"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>13</v>
-      </c>
-      <c r="B100" t="s">
-        <v>62</v>
-      </c>
-      <c r="C100" t="s">
-        <v>14</v>
-      </c>
-      <c r="D100" t="s">
-        <v>18</v>
-      </c>
-      <c r="F100" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>13</v>
-      </c>
-      <c r="B101" t="s">
-        <v>55</v>
-      </c>
-      <c r="C101" t="s">
-        <v>14</v>
-      </c>
-      <c r="D101" t="s">
-        <v>64</v>
-      </c>
+      <c r="F101" s="2"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>13</v>
       </c>
       <c r="B102" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C102" t="s">
         <v>14</v>
       </c>
       <c r="D102" t="s">
-        <v>64</v>
+        <v>18</v>
+      </c>
+      <c r="F102" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -2187,7 +2198,7 @@
         <v>13</v>
       </c>
       <c r="B103" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C103" t="s">
         <v>14</v>
@@ -2201,29 +2212,27 @@
         <v>13</v>
       </c>
       <c r="B104" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="C104" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="D104" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C105" s="2"/>
-      <c r="D105" s="2"/>
-      <c r="E105" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>68</v>
+      <c r="A105" t="s">
+        <v>13</v>
+      </c>
+      <c r="B105" t="s">
+        <v>63</v>
+      </c>
+      <c r="C105" t="s">
+        <v>14</v>
+      </c>
+      <c r="D105" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -2231,27 +2240,29 @@
         <v>13</v>
       </c>
       <c r="B106" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C106" t="s">
-        <v>14</v>
-      </c>
-      <c r="F106" t="s">
-        <v>21</v>
+        <v>66</v>
+      </c>
+      <c r="D106" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>13</v>
-      </c>
-      <c r="B107" t="s">
-        <v>55</v>
-      </c>
-      <c r="C107" t="s">
-        <v>14</v>
-      </c>
-      <c r="F107" s="12" t="s">
-        <v>72</v>
+      <c r="A107" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
@@ -2259,22 +2270,27 @@
         <v>13</v>
       </c>
       <c r="B108" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C108" t="s">
         <v>14</v>
       </c>
-      <c r="F108" s="12"/>
+      <c r="F108" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>13</v>
       </c>
       <c r="B109" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C109" t="s">
         <v>14</v>
+      </c>
+      <c r="F109" s="12" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
@@ -2282,60 +2298,49 @@
         <v>13</v>
       </c>
       <c r="B110" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="C110" t="s">
-        <v>66</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F110" s="12"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C111" s="2"/>
-      <c r="D111" s="2"/>
-      <c r="E111" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>68</v>
+      <c r="A111" t="s">
+        <v>13</v>
+      </c>
+      <c r="B111" t="s">
+        <v>63</v>
+      </c>
+      <c r="C111" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B112" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C112" t="s">
-        <v>14</v>
-      </c>
-      <c r="D112" t="s">
-        <v>52</v>
-      </c>
-      <c r="F112" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>28</v>
-      </c>
-      <c r="B113" t="s">
-        <v>55</v>
-      </c>
-      <c r="C113" t="s">
-        <v>14</v>
-      </c>
-      <c r="D113" t="s">
-        <v>27</v>
-      </c>
-      <c r="F113" t="s">
-        <v>88</v>
+      <c r="A113" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -2343,13 +2348,16 @@
         <v>28</v>
       </c>
       <c r="B114" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C114" t="s">
         <v>14</v>
       </c>
       <c r="D114" t="s">
-        <v>27</v>
+        <v>52</v>
+      </c>
+      <c r="F114" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -2357,77 +2365,77 @@
         <v>28</v>
       </c>
       <c r="B115" t="s">
+        <v>55</v>
+      </c>
+      <c r="C115" t="s">
+        <v>14</v>
+      </c>
+      <c r="D115" t="s">
+        <v>27</v>
+      </c>
+      <c r="F115" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>28</v>
+      </c>
+      <c r="B116" t="s">
+        <v>42</v>
+      </c>
+      <c r="C116" t="s">
+        <v>14</v>
+      </c>
+      <c r="D116" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>28</v>
+      </c>
+      <c r="B117" t="s">
         <v>63</v>
       </c>
-      <c r="C115" t="s">
-        <v>14</v>
-      </c>
-      <c r="D115" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" s="10" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A116" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B116" s="10" t="s">
+      <c r="C117" t="s">
+        <v>14</v>
+      </c>
+      <c r="D117" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" s="9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A118" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B118" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C116" s="10" t="s">
+      <c r="C118" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D116" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F116" s="11" t="s">
+      <c r="D118" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F118" s="10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117" s="2" t="s">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B119" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C117" s="2"/>
-      <c r="D117" s="2"/>
-      <c r="E117" s="2" t="s">
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F117" s="2" t="s">
+      <c r="F119" s="2" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>28</v>
-      </c>
-      <c r="B118" t="s">
-        <v>62</v>
-      </c>
-      <c r="C118" t="s">
-        <v>14</v>
-      </c>
-      <c r="D118" t="s">
-        <v>27</v>
-      </c>
-      <c r="F118" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>28</v>
-      </c>
-      <c r="B119" t="s">
-        <v>55</v>
-      </c>
-      <c r="C119" t="s">
-        <v>14</v>
-      </c>
-      <c r="D119" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -2435,13 +2443,16 @@
         <v>28</v>
       </c>
       <c r="B120" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C120" t="s">
         <v>14</v>
       </c>
       <c r="D120" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="F120" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -2449,7 +2460,7 @@
         <v>28</v>
       </c>
       <c r="B121" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C121" t="s">
         <v>14</v>
@@ -2463,29 +2474,27 @@
         <v>28</v>
       </c>
       <c r="B122" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="C122" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="D122" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A123" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C123" s="2"/>
-      <c r="D123" s="2"/>
-      <c r="E123" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>68</v>
+      <c r="A123" t="s">
+        <v>28</v>
+      </c>
+      <c r="B123" t="s">
+        <v>63</v>
+      </c>
+      <c r="C123" t="s">
+        <v>14</v>
+      </c>
+      <c r="D123" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
@@ -2493,41 +2502,72 @@
         <v>28</v>
       </c>
       <c r="B124" t="s">
+        <v>65</v>
+      </c>
+      <c r="C124" t="s">
+        <v>66</v>
+      </c>
+      <c r="D124" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C125" s="2"/>
+      <c r="D125" s="2"/>
+      <c r="E125" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>28</v>
+      </c>
+      <c r="B126" t="s">
         <v>62</v>
       </c>
-      <c r="C124" t="s">
-        <v>14</v>
-      </c>
-      <c r="D124" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F124" t="s">
+      <c r="C126" t="s">
+        <v>14</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F126" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A125" s="5" t="s">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B125" s="5" t="s">
+      <c r="B127" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C125" s="5" t="s">
+      <c r="C127" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D125" s="6" t="s">
+      <c r="D127" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E125" s="5" t="s">
+      <c r="E127" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F125" s="5"/>
+      <c r="F127" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="F84:F85"/>
-    <mergeCell ref="F107:F108"/>
+  <mergeCells count="4">
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="F109:F110"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>